<commit_message>
exportando dados do ithink para o excel para testar a adequação do modelo no R
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/rodada1/params_rodada1.xlsx
+++ b/models/dissertation-model/modelo-R/rodada1/params_rodada1.xlsx
@@ -940,7 +940,7 @@
   <dimension ref="A1:AMI60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
     <col min="7" max="7" width="10.85546875" style="1"/>
     <col min="8" max="8" width="11" style="1"/>
     <col min="9" max="9" width="7.28515625" style="1"/>
-    <col min="10" max="10" width="10.85546875" style="1"/>
+    <col min="10" max="10" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="1"/>
     <col min="12" max="12" width="10.42578125" style="1"/>
     <col min="13" max="13" width="10" style="1"/>

</xml_diff>